<commit_message>
final add for nov30
</commit_message>
<xml_diff>
--- a/timeTrackerOffsetDesign.xlsx
+++ b/timeTrackerOffsetDesign.xlsx
@@ -402,7 +402,7 @@
       </c>
       <c r="B1" s="6" t="n">
         <f aca="false">SUM(M5:M100)</f>
-        <v>11</v>
+        <v>11.25</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -604,15 +604,15 @@
         <v>44165</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="L8" s="12" t="n">
         <f aca="false">SUM(B8:K8)</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="M8" s="3" t="n">
         <f aca="false">L8/60</f>
-        <v>1</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated code for tablets (<1450px)
</commit_message>
<xml_diff>
--- a/timeTrackerOffsetDesign.xlsx
+++ b/timeTrackerOffsetDesign.xlsx
@@ -153,7 +153,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mmm\ d&quot;, &quot;yyyy"/>
-    <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -247,7 +247,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,6 +264,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,7 +280,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -382,7 +394,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,191 +403,192 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="2" width="9.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="2" width="9.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="3" width="11.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="14" style="4" width="17.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="30" style="4" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="11.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="4" width="11.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="14" style="5" width="17.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="30" style="5" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="n">
+    <row r="1" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="n">
         <f aca="false">SUM(M5:M100)</f>
-        <v>11.25</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-    </row>
-    <row r="2" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-    </row>
-    <row r="3" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+        <v>12.8333333333333</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+    </row>
+    <row r="2" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+    </row>
+    <row r="3" s="12" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="L4" s="12"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="n">
+      <c r="A5" s="13" t="n">
         <v>44160</v>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="14" t="n">
         <v>210</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11" t="n">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14" t="n">
         <v>60</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12" t="n">
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="15" t="n">
         <f aca="false">SUM(B5:K5)</f>
         <v>270</v>
       </c>
-      <c r="M5" s="3" t="n">
+      <c r="M5" s="4" t="n">
         <f aca="false">L5/60</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="13" t="n">
         <v>44161</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="H6" s="11" t="n">
+      <c r="D6" s="14"/>
+      <c r="H6" s="14" t="n">
         <v>30</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="12" t="n">
+      <c r="I6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="15" t="n">
         <f aca="false">SUM(B6:K6)</f>
         <v>30</v>
       </c>
-      <c r="M6" s="3" t="n">
+      <c r="M6" s="4" t="n">
         <f aca="false">L6/60</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="13" t="n">
         <v>44162</v>
       </c>
       <c r="C7" s="2" t="n">
@@ -590,302 +603,310 @@
       <c r="I7" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="L7" s="12" t="n">
+      <c r="L7" s="15" t="n">
         <f aca="false">SUM(B7:K7)</f>
         <v>300</v>
       </c>
-      <c r="M7" s="3" t="n">
+      <c r="M7" s="4" t="n">
         <f aca="false">L7/60</f>
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="13" t="n">
         <v>44165</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>75</v>
       </c>
-      <c r="L8" s="12" t="n">
+      <c r="I8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L8" s="15" t="n">
         <f aca="false">SUM(B8:K8)</f>
-        <v>75</v>
-      </c>
-      <c r="M8" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="M8" s="4" t="n">
         <f aca="false">L8/60</f>
-        <v>1.25</v>
+        <v>1.33333333333333</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="L9" s="12" t="n">
+      <c r="A9" s="13" t="n">
+        <v>44166</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>90</v>
+      </c>
+      <c r="L9" s="15" t="n">
         <f aca="false">SUM(B9:K9)</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="M9" s="4" t="n">
         <f aca="false">L9/60</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="L10" s="12" t="n">
+      <c r="A10" s="13"/>
+      <c r="L10" s="15" t="n">
         <f aca="false">SUM(B10:K10)</f>
         <v>0</v>
       </c>
-      <c r="M10" s="3" t="n">
+      <c r="M10" s="4" t="n">
         <f aca="false">L10/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
-      <c r="L11" s="12" t="n">
+      <c r="A11" s="13"/>
+      <c r="L11" s="15" t="n">
         <f aca="false">SUM(B11:K11)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="3" t="n">
+      <c r="M11" s="4" t="n">
         <f aca="false">L11/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-      <c r="L12" s="12" t="n">
+      <c r="A12" s="13"/>
+      <c r="L12" s="15" t="n">
         <f aca="false">SUM(B12:K12)</f>
         <v>0</v>
       </c>
-      <c r="M12" s="3" t="n">
+      <c r="M12" s="4" t="n">
         <f aca="false">L12/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10"/>
-      <c r="L13" s="12" t="n">
+      <c r="A13" s="13"/>
+      <c r="L13" s="15" t="n">
         <f aca="false">SUM(B13:K13)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="3" t="n">
+      <c r="M13" s="4" t="n">
         <f aca="false">L13/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10"/>
-      <c r="L14" s="12" t="n">
+      <c r="A14" s="13"/>
+      <c r="L14" s="15" t="n">
         <f aca="false">SUM(B14:K14)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="3" t="n">
+      <c r="M14" s="4" t="n">
         <f aca="false">L14/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10"/>
-      <c r="L15" s="12" t="n">
+      <c r="A15" s="13"/>
+      <c r="L15" s="15" t="n">
         <f aca="false">SUM(B15:K15)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="3" t="n">
+      <c r="M15" s="4" t="n">
         <f aca="false">L15/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
-      <c r="L16" s="12" t="n">
+      <c r="A16" s="13"/>
+      <c r="L16" s="15" t="n">
         <f aca="false">SUM(B16:K16)</f>
         <v>0</v>
       </c>
-      <c r="M16" s="3" t="n">
+      <c r="M16" s="4" t="n">
         <f aca="false">L16/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
-      <c r="L17" s="12" t="n">
+      <c r="A17" s="13"/>
+      <c r="L17" s="15" t="n">
         <f aca="false">SUM(B17:K17)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="3" t="n">
+      <c r="M17" s="4" t="n">
         <f aca="false">L17/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
-      <c r="L18" s="12" t="n">
+      <c r="A18" s="13"/>
+      <c r="L18" s="15" t="n">
         <f aca="false">SUM(B18:K18)</f>
         <v>0</v>
       </c>
-      <c r="M18" s="3" t="n">
+      <c r="M18" s="4" t="n">
         <f aca="false">L18/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10"/>
-      <c r="L19" s="12" t="n">
+      <c r="A19" s="13"/>
+      <c r="L19" s="15" t="n">
         <f aca="false">SUM(B19:K19)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="3" t="n">
+      <c r="M19" s="4" t="n">
         <f aca="false">L19/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10"/>
-      <c r="L20" s="12" t="n">
+      <c r="A20" s="13"/>
+      <c r="L20" s="15" t="n">
         <f aca="false">SUM(B20:K20)</f>
         <v>0</v>
       </c>
-      <c r="M20" s="3" t="n">
+      <c r="M20" s="4" t="n">
         <f aca="false">L20/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10"/>
-      <c r="L21" s="12" t="n">
+      <c r="A21" s="13"/>
+      <c r="L21" s="15" t="n">
         <f aca="false">SUM(B21:K21)</f>
         <v>0</v>
       </c>
-      <c r="M21" s="3" t="n">
+      <c r="M21" s="4" t="n">
         <f aca="false">L21/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10"/>
-      <c r="L22" s="12" t="n">
+      <c r="A22" s="13"/>
+      <c r="L22" s="15" t="n">
         <f aca="false">SUM(B22:K22)</f>
         <v>0</v>
       </c>
-      <c r="M22" s="3" t="n">
+      <c r="M22" s="4" t="n">
         <f aca="false">L22/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10"/>
-      <c r="L23" s="12" t="n">
+      <c r="A23" s="13"/>
+      <c r="L23" s="15" t="n">
         <f aca="false">SUM(B23:K23)</f>
         <v>0</v>
       </c>
-      <c r="M23" s="3" t="n">
+      <c r="M23" s="4" t="n">
         <f aca="false">L23/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10"/>
-      <c r="L24" s="12" t="n">
+      <c r="A24" s="13"/>
+      <c r="L24" s="15" t="n">
         <f aca="false">SUM(B24:K24)</f>
         <v>0</v>
       </c>
-      <c r="M24" s="3" t="n">
+      <c r="M24" s="4" t="n">
         <f aca="false">L24/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10"/>
-      <c r="L25" s="12" t="n">
+      <c r="A25" s="13"/>
+      <c r="L25" s="15" t="n">
         <f aca="false">SUM(B25:K25)</f>
         <v>0</v>
       </c>
-      <c r="M25" s="3" t="n">
+      <c r="M25" s="4" t="n">
         <f aca="false">L25/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10"/>
-      <c r="L26" s="12" t="n">
+      <c r="A26" s="13"/>
+      <c r="L26" s="15" t="n">
         <f aca="false">SUM(B26:K26)</f>
         <v>0</v>
       </c>
-      <c r="M26" s="3" t="n">
+      <c r="M26" s="4" t="n">
         <f aca="false">L26/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10"/>
-      <c r="L27" s="12" t="n">
+      <c r="A27" s="13"/>
+      <c r="L27" s="15" t="n">
         <f aca="false">SUM(B27:K27)</f>
         <v>0</v>
       </c>
-      <c r="M27" s="3" t="n">
+      <c r="M27" s="4" t="n">
         <f aca="false">L27/60</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10"/>
+      <c r="A28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10"/>
+      <c r="A29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
+      <c r="A30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10"/>
+      <c r="A31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10"/>
+      <c r="A32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10"/>
+      <c r="A33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10"/>
+      <c r="A34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10"/>
+      <c r="A35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10"/>
+      <c r="A36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10"/>
+      <c r="A37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10"/>
+      <c r="A38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10"/>
+      <c r="A39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10"/>
+      <c r="A40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10"/>
+      <c r="A41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10"/>
+      <c r="A42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10"/>
+      <c r="A43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10"/>
+      <c r="A44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10"/>
+      <c r="A45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10"/>
+      <c r="A46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="10"/>
+      <c r="A47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10"/>
+      <c r="A48" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
worked on portfolio section
</commit_message>
<xml_diff>
--- a/timeTrackerOffsetDesign.xlsx
+++ b/timeTrackerOffsetDesign.xlsx
@@ -394,7 +394,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -415,7 +415,7 @@
       </c>
       <c r="B1" s="7" t="n">
         <f aca="false">SUM(M5:M100)</f>
-        <v>12.8333333333333</v>
+        <v>16.25</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -648,25 +648,38 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
+      <c r="A10" s="13" t="n">
+        <v>44168</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>60</v>
+      </c>
       <c r="L10" s="15" t="n">
         <f aca="false">SUM(B10:K10)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M10" s="4" t="n">
         <f aca="false">L10/60</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
+      <c r="A11" s="13" t="n">
+        <v>44173</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>135</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>10</v>
+      </c>
       <c r="L11" s="15" t="n">
         <f aca="false">SUM(B11:K11)</f>
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="M11" s="4" t="n">
         <f aca="false">L11/60</f>
-        <v>0</v>
+        <v>2.41666666666667</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated after talk with client on Dec 8
</commit_message>
<xml_diff>
--- a/timeTrackerOffsetDesign.xlsx
+++ b/timeTrackerOffsetDesign.xlsx
@@ -394,7 +394,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -415,7 +415,7 @@
       </c>
       <c r="B1" s="7" t="n">
         <f aca="false">SUM(M5:M100)</f>
-        <v>16.25</v>
+        <v>19</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -683,25 +683,35 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
+      <c r="A12" s="13" t="n">
+        <v>44178</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>45</v>
+      </c>
       <c r="L12" s="15" t="n">
         <f aca="false">SUM(B12:K12)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="M12" s="4" t="n">
         <f aca="false">L12/60</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
+      <c r="A13" s="13" t="n">
+        <v>44181</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>120</v>
+      </c>
       <c r="L13" s="15" t="n">
         <f aca="false">SUM(B13:K13)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M13" s="4" t="n">
         <f aca="false">L13/60</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added favicon to work
</commit_message>
<xml_diff>
--- a/timeTrackerOffsetDesign.xlsx
+++ b/timeTrackerOffsetDesign.xlsx
@@ -394,7 +394,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -415,7 +415,7 @@
       </c>
       <c r="B1" s="7" t="n">
         <f aca="false">SUM(M5:M100)</f>
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -703,15 +703,15 @@
         <v>44181</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="L13" s="15" t="n">
         <f aca="false">SUM(B13:K13)</f>
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="M13" s="4" t="n">
         <f aca="false">L13/60</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixed title alignement in about section
</commit_message>
<xml_diff>
--- a/timeTrackerOffsetDesign.xlsx
+++ b/timeTrackerOffsetDesign.xlsx
@@ -394,7 +394,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -415,7 +415,7 @@
       </c>
       <c r="B1" s="7" t="n">
         <f aca="false">SUM(M5:M100)</f>
-        <v>19.5</v>
+        <v>21.25</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -715,14 +715,19 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
+      <c r="A14" s="13" t="n">
+        <v>44207</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>105</v>
+      </c>
       <c r="L14" s="15" t="n">
         <f aca="false">SUM(B14:K14)</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="M14" s="4" t="n">
         <f aca="false">L14/60</f>
-        <v>0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>